<commit_message>
edit load test function edit qa test
</commit_message>
<xml_diff>
--- a/QA/checkListUserInteract.xlsx
+++ b/QA/checkListUserInteract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zork/Desktop/swift/StoreRoom/QA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9D98E7-516B-1F46-8781-14CE41D038CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D106501-8370-734C-8256-0F777A837A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{1750086F-CB51-6142-916C-E63E7E47E19E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Проект</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>1.0.1</t>
+  </si>
+  <si>
+    <t>Приложение переключилось на ландшафтную ориентацию. При ландшафтной ориентации приложение не выполняет основные функции. Ландшафтная ориентация не предусмотрена ТЗ.</t>
+  </si>
+  <si>
+    <t>Плавность скроллинга</t>
+  </si>
+  <si>
+    <t>При скроллинге более 10 элементов видно затормаживание</t>
   </si>
 </sst>
 </file>
@@ -613,7 +622,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,7 +718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -717,7 +726,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -728,7 +740,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -739,7 +751,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -750,14 +762,22 @@
         <v>22</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="8">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -768,7 +788,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C9:C12">
+  <conditionalFormatting sqref="C9:C13">
     <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="skipped">
       <formula>NOT(ISERROR(SEARCH("skipped",C9)))</formula>
     </cfRule>
@@ -795,6 +815,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -802,7 +823,7 @@
           <x14:formula1>
             <xm:f>данные!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:C12</xm:sqref>
+          <xm:sqref>C9:C13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>